<commit_message>
Update samples Excel file
</commit_message>
<xml_diff>
--- a/samples.xlsx
+++ b/samples.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dennis/vsCode/Python-Test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dennis/vsCode/PP3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C94712E-7236-CA41-9C46-C9EFAB9DC122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5C246B-2504-8749-B9AD-920AFFBC688F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5080" yWindow="3100" windowWidth="28240" windowHeight="17240" xr2:uid="{62BEFB82-1EE4-9C41-9C02-77936C8E147B}"/>
+    <workbookView xWindow="6440" yWindow="4620" windowWidth="28240" windowHeight="17240" xr2:uid="{62BEFB82-1EE4-9C41-9C02-77936C8E147B}"/>
   </bookViews>
   <sheets>
     <sheet name="samples_1" sheetId="1" r:id="rId1"/>
@@ -36,17 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Row 1</t>
   </si>
   <si>
-    <t>Row 2</t>
-  </si>
-  <si>
-    <t>Row 3</t>
-  </si>
-  <si>
     <t>Jack</t>
   </si>
   <si>
@@ -68,7 +62,28 @@
     <t>Dan</t>
   </si>
   <si>
-    <t>no</t>
+    <t>How motivated are you to come to work every day?</t>
+  </si>
+  <si>
+    <t>How much do you feel valued and recognized for your work?</t>
+  </si>
+  <si>
+    <t>How would you rate the opportunities for professional development and career opportunities in the company?</t>
+  </si>
+  <si>
+    <t>Do you feel you are treated fairly and equally?</t>
+  </si>
+  <si>
+    <t>How would you rate the company's salary and benefits?</t>
+  </si>
+  <si>
+    <t>How transparent are decision-making processes in the company?</t>
+  </si>
+  <si>
+    <t>How would you rate the leadership skills in the company?</t>
+  </si>
+  <si>
+    <t>How well are new employees integrated into the company?</t>
   </si>
 </sst>
 </file>
@@ -104,8 +119,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -420,100 +438,247 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BA33832-65A5-6A4C-9C2B-05766E1D9E96}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="9" width="12.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>6</v>
+      </c>
+      <c r="H6">
+        <v>7</v>
+      </c>
+      <c r="I6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>7</v>
+      </c>
+      <c r="I7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
-        <v>10</v>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="I8">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bring data from Excel and G-Sheet into same format
</commit_message>
<xml_diff>
--- a/samples.xlsx
+++ b/samples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dennis/vsCode/PP3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5C246B-2504-8749-B9AD-920AFFBC688F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27763055-1B1D-1345-9EC9-6FF4D68981FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6440" yWindow="4620" windowWidth="28240" windowHeight="17240" xr2:uid="{62BEFB82-1EE4-9C41-9C02-77936C8E147B}"/>
   </bookViews>
@@ -38,52 +38,52 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
-    <t>Row 1</t>
-  </si>
-  <si>
-    <t>Jack</t>
+    <t>How motivated are you to come to work every day?</t>
+  </si>
+  <si>
+    <t>How much do you feel valued and recognized for your work?</t>
+  </si>
+  <si>
+    <t>How would you rate the opportunities for professional development and career opportunities in the company?</t>
+  </si>
+  <si>
+    <t>Do you feel you are treated fairly and equally?</t>
+  </si>
+  <si>
+    <t>How would you rate the company's salary and benefits?</t>
+  </si>
+  <si>
+    <t>How transparent are decision-making processes in the company?</t>
+  </si>
+  <si>
+    <t>How would you rate the leadership skills in the company?</t>
+  </si>
+  <si>
+    <t>How well are new employees integrated into the company?</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Dirk</t>
+  </si>
+  <si>
+    <t>Anna</t>
   </si>
   <si>
     <t>Marie</t>
   </si>
   <si>
-    <t>Martin</t>
-  </si>
-  <si>
-    <t>Tom</t>
-  </si>
-  <si>
-    <t>Vanessa</t>
-  </si>
-  <si>
-    <t>Ylvi</t>
-  </si>
-  <si>
-    <t>Dan</t>
-  </si>
-  <si>
-    <t>How motivated are you to come to work every day?</t>
-  </si>
-  <si>
-    <t>How much do you feel valued and recognized for your work?</t>
-  </si>
-  <si>
-    <t>How would you rate the opportunities for professional development and career opportunities in the company?</t>
-  </si>
-  <si>
-    <t>Do you feel you are treated fairly and equally?</t>
-  </si>
-  <si>
-    <t>How would you rate the company's salary and benefits?</t>
-  </si>
-  <si>
-    <t>How transparent are decision-making processes in the company?</t>
-  </si>
-  <si>
-    <t>How would you rate the leadership skills in the company?</t>
-  </si>
-  <si>
-    <t>How well are new employees integrated into the company?</t>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Stephanie</t>
+  </si>
+  <si>
+    <t>Laura</t>
   </si>
 </sst>
 </file>
@@ -441,7 +441,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="A8" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -451,39 +451,39 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
       </c>
       <c r="C2">
         <v>6</v>
@@ -508,11 +508,11 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
       </c>
       <c r="C3">
         <v>7</v>
@@ -537,11 +537,11 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -566,11 +566,11 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
         <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
       </c>
       <c r="C5">
         <v>6</v>
@@ -595,11 +595,11 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>9</v>
       </c>
       <c r="C6">
         <v>6</v>
@@ -624,10 +624,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
       <c r="C7">
@@ -653,11 +653,11 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
       </c>
       <c r="C8">
         <v>9</v>
@@ -683,5 +683,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Extend Excel file structure
</commit_message>
<xml_diff>
--- a/samples.xlsx
+++ b/samples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dennis/vsCode/PP3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27763055-1B1D-1345-9EC9-6FF4D68981FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8C1E4F-4E92-D54F-B90D-21BB5CE95E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6440" yWindow="4620" windowWidth="28240" windowHeight="17240" xr2:uid="{62BEFB82-1EE4-9C41-9C02-77936C8E147B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>How motivated are you to come to work every day?</t>
   </si>
@@ -84,16 +84,35 @@
   </si>
   <si>
     <t>Laura</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>MadeUp Inc.</t>
+  </si>
+  <si>
+    <t>What A Corp.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -119,11 +138,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -142,9 +163,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -182,7 +203,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -288,7 +309,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -430,7 +451,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -438,246 +459,294 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BA33832-65A5-6A4C-9C2B-05766E1D9E96}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A2:A8"/>
+      <selection activeCell="A7" sqref="A1:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="9" width="12.6640625" customWidth="1"/>
+    <col min="4" max="11" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>45137</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>6</v>
+      <c r="C2" t="s">
+        <v>18</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2">
         <v>4</v>
       </c>
       <c r="G2">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
         <v>3</v>
       </c>
-      <c r="H2">
-        <v>6</v>
-      </c>
-      <c r="I2">
+      <c r="J2">
+        <v>6</v>
+      </c>
+      <c r="K2">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>45140</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
+      <c r="C3" t="s">
+        <v>19</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3">
         <v>5</v>
       </c>
       <c r="G3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H3">
         <v>5</v>
       </c>
       <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <v>5</v>
+      </c>
+      <c r="K3">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>45141</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
+      <c r="C4" t="s">
+        <v>18</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
         <v>9</v>
       </c>
-      <c r="F4">
-        <v>6</v>
-      </c>
-      <c r="G4">
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="I4">
         <v>2</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>3</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>45145</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>6</v>
+      <c r="C5" t="s">
+        <v>18</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
       <c r="E5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
         <v>1</v>
       </c>
-      <c r="H5">
-        <v>5</v>
-      </c>
-      <c r="I5">
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>45160</v>
+      </c>
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="B6">
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
         <v>9</v>
       </c>
-      <c r="C6">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>6</v>
-      </c>
       <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6">
         <v>9</v>
       </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <v>6</v>
-      </c>
       <c r="H6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <v>7</v>
+      </c>
+      <c r="K6">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>45179</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>8</v>
+      <c r="C7" t="s">
+        <v>19</v>
       </c>
       <c r="D7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E7">
         <v>8</v>
       </c>
       <c r="F7">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H7">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>7</v>
+      </c>
+      <c r="K7">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>45186</v>
+      </c>
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="B8">
-        <v>4</v>
-      </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
         <v>9</v>
       </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-      <c r="E8">
-        <v>7</v>
-      </c>
       <c r="F8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G8">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="J8">
+        <v>6</v>
+      </c>
+      <c r="K8">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix data formating from excel and g-spread
</commit_message>
<xml_diff>
--- a/samples.xlsx
+++ b/samples.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dennis/vsCode/PP3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dennis/Development/Code/PP3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8C1E4F-4E92-D54F-B90D-21BB5CE95E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEC966A-F2E1-514E-85E6-C4DC57B705F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6440" yWindow="4620" windowWidth="28240" windowHeight="17240" xr2:uid="{62BEFB82-1EE4-9C41-9C02-77936C8E147B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>How motivated are you to come to work every day?</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>What A Corp.</t>
+  </si>
+  <si>
+    <t>Employees Dream Inc.</t>
   </si>
 </sst>
 </file>
@@ -163,9 +166,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -203,7 +206,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -309,7 +312,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -451,7 +454,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -462,7 +465,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A1:K8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -618,7 +621,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -723,7 +726,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <v>4</v>

</xml_diff>

<commit_message>
Shorten question in Excel file samples.xlsx
</commit_message>
<xml_diff>
--- a/samples.xlsx
+++ b/samples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dennis/Development/Code/PP3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEC966A-F2E1-514E-85E6-C4DC57B705F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A39CF2-835F-874F-A468-F514F3024EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6440" yWindow="4620" windowWidth="28240" windowHeight="17240" xr2:uid="{62BEFB82-1EE4-9C41-9C02-77936C8E147B}"/>
   </bookViews>
@@ -44,9 +44,6 @@
     <t>How much do you feel valued and recognized for your work?</t>
   </si>
   <si>
-    <t>How would you rate the opportunities for professional development and career opportunities in the company?</t>
-  </si>
-  <si>
     <t>Do you feel you are treated fairly and equally?</t>
   </si>
   <si>
@@ -99,13 +96,16 @@
   </si>
   <si>
     <t>Employees Dream Inc.</t>
+  </si>
+  <si>
+    <t>How are the opportunities for development and career in the company?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -119,6 +119,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -143,11 +149,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -166,9 +170,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -206,7 +210,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -312,7 +316,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -454,7 +458,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -465,7 +469,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -475,48 +479,48 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>7</v>
+      <c r="I1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>45137</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2">
         <v>7</v>
@@ -544,14 +548,14 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>45140</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3">
         <v>6</v>
@@ -579,14 +583,14 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>45141</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4">
         <v>8</v>
@@ -614,14 +618,14 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>45145</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -649,14 +653,14 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>45160</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6">
         <v>9</v>
@@ -684,14 +688,14 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>45179</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7">
         <v>6</v>
@@ -719,14 +723,14 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>45186</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8">
         <v>4</v>

</xml_diff>